<commit_message>
create App and work authorization
</commit_message>
<xml_diff>
--- a/DataDictionary.xlsx
+++ b/DataDictionary.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24332"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A618FEEF-F49B-4542-BB53-5F35D6683C6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF64F1C7-132C-4567-A956-13D29E771E37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9036" yWindow="1704" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataDictionary" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="73">
   <si>
     <t>Data Dictionary</t>
   </si>
@@ -145,12 +145,6 @@
     <t>NVARCHAR(15)</t>
   </si>
   <si>
-    <t>Owner</t>
-  </si>
-  <si>
-    <t>OwnerID</t>
-  </si>
-  <si>
     <t>Foreign Key to Adress</t>
   </si>
   <si>
@@ -163,9 +157,6 @@
     <t>MidleName</t>
   </si>
   <si>
-    <t>Foreign Key to Owner</t>
-  </si>
-  <si>
     <t>Foreign Key to Model</t>
   </si>
   <si>
@@ -190,9 +181,6 @@
     <t>NVARCHAR(50)</t>
   </si>
   <si>
-    <t>NVARCHAR(30)</t>
-  </si>
-  <si>
     <t>Car</t>
   </si>
   <si>
@@ -203,6 +191,51 @@
   </si>
   <si>
     <t>Номер Осаго</t>
+  </si>
+  <si>
+    <t>ColorID</t>
+  </si>
+  <si>
+    <t>Person</t>
+  </si>
+  <si>
+    <t>PersonID</t>
+  </si>
+  <si>
+    <t>Foreign Key to Person</t>
+  </si>
+  <si>
+    <t>Foreign Ket to Color</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>UserID</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>NVARCHAR(320)</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>RoleID</t>
+  </si>
+  <si>
+    <t>Foreign Key to Role</t>
+  </si>
+  <si>
+    <t>Role</t>
+  </si>
+  <si>
+    <t>NVARCHAR(3)</t>
   </si>
 </sst>
 </file>
@@ -415,7 +448,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -477,6 +510,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -495,25 +549,7 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -883,10 +919,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:E58"/>
+  <dimension ref="A1:E77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E52" sqref="E52"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C72" sqref="C72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4"/>
@@ -900,29 +936,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="4" customFormat="1" ht="31.5" customHeight="1">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
     </row>
     <row r="2" spans="1:5" s="4" customFormat="1" ht="24" customHeight="1">
-      <c r="A2" s="22"/>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
+      <c r="A2" s="29"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
     </row>
     <row r="4" spans="1:5" ht="21.75" customHeight="1">
-      <c r="A4" s="23" t="s">
+      <c r="A4" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="23"/>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="23"/>
+      <c r="B4" s="30"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
     </row>
     <row r="5" spans="1:5" ht="20.25" customHeight="1">
       <c r="A5" s="6" t="s">
@@ -979,13 +1015,13 @@
       <c r="E8" s="10"/>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="23" t="s">
+      <c r="A9" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="23"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="23"/>
+      <c r="B9" s="30"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="30"/>
+      <c r="E9" s="30"/>
     </row>
     <row r="10" spans="1:5" ht="28.8">
       <c r="A10" s="6" t="s">
@@ -1052,20 +1088,20 @@
       </c>
     </row>
     <row r="14" spans="1:5" ht="15.6" customHeight="1">
-      <c r="A14" s="32"/>
+      <c r="A14" s="23"/>
       <c r="B14" s="15"/>
       <c r="C14" s="16"/>
       <c r="D14" s="14"/>
       <c r="E14" s="10"/>
     </row>
     <row r="15" spans="1:5" ht="20.25" customHeight="1">
-      <c r="A15" s="24" t="s">
+      <c r="A15" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="25"/>
-      <c r="C15" s="25"/>
-      <c r="D15" s="25"/>
-      <c r="E15" s="26"/>
+      <c r="B15" s="32"/>
+      <c r="C15" s="32"/>
+      <c r="D15" s="32"/>
+      <c r="E15" s="33"/>
     </row>
     <row r="16" spans="1:5" ht="28.8">
       <c r="A16" s="6" t="s">
@@ -1122,13 +1158,13 @@
       <c r="E19" s="10"/>
     </row>
     <row r="20" spans="1:5" ht="21.75" customHeight="1">
-      <c r="A20" s="27" t="s">
+      <c r="A20" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="B20" s="28"/>
-      <c r="C20" s="28"/>
-      <c r="D20" s="28"/>
-      <c r="E20" s="29"/>
+      <c r="B20" s="26"/>
+      <c r="C20" s="26"/>
+      <c r="D20" s="26"/>
+      <c r="E20" s="27"/>
     </row>
     <row r="21" spans="1:5" ht="20.25" customHeight="1">
       <c r="A21" s="11" t="s">
@@ -1202,13 +1238,13 @@
       <c r="E25" s="10"/>
     </row>
     <row r="26" spans="1:5" ht="21.75" customHeight="1">
-      <c r="A26" s="27" t="s">
+      <c r="A26" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="B26" s="28"/>
-      <c r="C26" s="28"/>
-      <c r="D26" s="28"/>
-      <c r="E26" s="29"/>
+      <c r="B26" s="26"/>
+      <c r="C26" s="26"/>
+      <c r="D26" s="26"/>
+      <c r="E26" s="27"/>
     </row>
     <row r="27" spans="1:5" ht="20.25" customHeight="1">
       <c r="A27" s="11" t="s">
@@ -1277,18 +1313,18 @@
     <row r="31" spans="1:5">
       <c r="A31" s="14"/>
       <c r="B31" s="15"/>
-      <c r="C31" s="30"/>
+      <c r="C31" s="21"/>
       <c r="D31" s="14"/>
-      <c r="E31" s="31"/>
+      <c r="E31" s="22"/>
     </row>
     <row r="32" spans="1:5">
-      <c r="A32" s="27" t="s">
+      <c r="A32" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="B32" s="28"/>
-      <c r="C32" s="28"/>
-      <c r="D32" s="28"/>
-      <c r="E32" s="29"/>
+      <c r="B32" s="26"/>
+      <c r="C32" s="26"/>
+      <c r="D32" s="26"/>
+      <c r="E32" s="27"/>
     </row>
     <row r="33" spans="1:5" ht="28.8">
       <c r="A33" s="11" t="s">
@@ -1325,53 +1361,53 @@
       </c>
     </row>
     <row r="35" spans="1:5" ht="20.25" customHeight="1">
-      <c r="A35" s="33"/>
+      <c r="A35" s="24"/>
       <c r="B35" s="3" t="s">
         <v>34</v>
       </c>
       <c r="C35" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D35" s="33" t="s">
+      <c r="D35" s="24" t="s">
         <v>7</v>
       </c>
       <c r="E35" s="3"/>
     </row>
     <row r="36" spans="1:5">
-      <c r="A36" s="33"/>
+      <c r="A36" s="24"/>
       <c r="B36" s="3" t="s">
         <v>35</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D36" s="33" t="s">
+      <c r="D36" s="24" t="s">
         <v>7</v>
       </c>
       <c r="E36" s="3"/>
     </row>
     <row r="37" spans="1:5">
-      <c r="A37" s="33"/>
+      <c r="A37" s="24"/>
       <c r="B37" s="3" t="s">
         <v>37</v>
       </c>
       <c r="C37" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D37" s="33" t="s">
+      <c r="D37" s="24" t="s">
         <v>7</v>
       </c>
       <c r="E37" s="3"/>
     </row>
     <row r="38" spans="1:5">
-      <c r="A38" s="33"/>
+      <c r="A38" s="24"/>
       <c r="B38" s="3" t="s">
         <v>32</v>
       </c>
       <c r="C38" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D38" s="33" t="s">
+      <c r="D38" s="24" t="s">
         <v>7</v>
       </c>
       <c r="E38" s="3" t="s">
@@ -1379,26 +1415,26 @@
       </c>
     </row>
     <row r="39" spans="1:5">
-      <c r="A39" s="33"/>
+      <c r="A39" s="24"/>
       <c r="B39" s="3" t="s">
         <v>40</v>
       </c>
       <c r="C39" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D39" s="33" t="s">
+      <c r="D39" s="24" t="s">
         <v>7</v>
       </c>
       <c r="E39" s="3"/>
     </row>
     <row r="41" spans="1:5">
-      <c r="A41" s="27" t="s">
-        <v>42</v>
-      </c>
-      <c r="B41" s="28"/>
-      <c r="C41" s="28"/>
-      <c r="D41" s="28"/>
-      <c r="E41" s="29"/>
+      <c r="A41" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="B41" s="26"/>
+      <c r="C41" s="26"/>
+      <c r="D41" s="26"/>
+      <c r="E41" s="27"/>
     </row>
     <row r="42" spans="1:5" ht="28.8">
       <c r="A42" s="11" t="s">
@@ -1422,7 +1458,7 @@
         <v>9</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
       <c r="C43" s="17" t="s">
         <v>11</v>
@@ -1435,46 +1471,46 @@
       </c>
     </row>
     <row r="44" spans="1:5">
-      <c r="A44" s="33"/>
+      <c r="A44" s="24"/>
       <c r="B44" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C44" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D44" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="E44" s="3"/>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" s="24"/>
+      <c r="B45" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="D44" s="33" t="s">
-        <v>7</v>
-      </c>
-      <c r="E44" s="3"/>
-    </row>
-    <row r="45" spans="1:5">
-      <c r="A45" s="33"/>
-      <c r="B45" s="3" t="s">
-        <v>47</v>
-      </c>
       <c r="C45" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="D45" s="33" t="s">
-        <v>46</v>
+        <v>43</v>
+      </c>
+      <c r="D45" s="24" t="s">
+        <v>44</v>
       </c>
       <c r="E45" s="3"/>
     </row>
     <row r="46" spans="1:5">
-      <c r="A46" s="33"/>
+      <c r="A46" s="24"/>
       <c r="B46" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="D46" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="D46" s="24" t="s">
         <v>7</v>
       </c>
       <c r="E46" s="3"/>
     </row>
     <row r="47" spans="1:5">
-      <c r="A47" s="33" t="s">
+      <c r="A47" s="24" t="s">
         <v>24</v>
       </c>
       <c r="B47" s="3" t="s">
@@ -1483,21 +1519,28 @@
       <c r="C47" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D47" s="33" t="s">
+      <c r="D47" s="24" t="s">
         <v>7</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>44</v>
-      </c>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48" s="34"/>
+      <c r="B48" s="22"/>
+      <c r="C48" s="22"/>
+      <c r="D48" s="34"/>
+      <c r="E48" s="22"/>
     </row>
     <row r="49" spans="1:5">
-      <c r="A49" s="27" t="s">
-        <v>58</v>
-      </c>
-      <c r="B49" s="28"/>
-      <c r="C49" s="28"/>
-      <c r="D49" s="28"/>
-      <c r="E49" s="29"/>
+      <c r="A49" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="B49" s="26"/>
+      <c r="C49" s="26"/>
+      <c r="D49" s="26"/>
+      <c r="E49" s="27"/>
     </row>
     <row r="50" spans="1:5" ht="28.8">
       <c r="A50" s="11" t="s">
@@ -1517,130 +1560,372 @@
       </c>
     </row>
     <row r="51" spans="1:5">
-      <c r="A51" s="8" t="s">
+      <c r="A51" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="B51" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="C51" s="17" t="s">
+      <c r="B51" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="C51" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="D51" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E51" s="18" t="s">
+      <c r="D51" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="E51" s="22" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="52" spans="1:5">
-      <c r="A52" s="33"/>
-      <c r="B52" s="3" t="s">
+      <c r="A52" s="34"/>
+      <c r="B52" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="C52" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="D52" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="E52" s="22"/>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53" s="34"/>
+      <c r="B53" s="22"/>
+      <c r="C53" s="22"/>
+      <c r="D53" s="34"/>
+      <c r="E53" s="22"/>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="B54" s="26"/>
+      <c r="C54" s="26"/>
+      <c r="D54" s="26"/>
+      <c r="E54" s="27"/>
+    </row>
+    <row r="55" spans="1:5" ht="28.8">
+      <c r="A55" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B55" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C55" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="D55" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="E55" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="B56" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="C56" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="D56" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="E56" s="22" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57" s="34"/>
+      <c r="B57" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="C57" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="D57" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="E57" s="22"/>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58" s="34"/>
+      <c r="B58" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="C58" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="D58" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="E58" s="22"/>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59" s="34"/>
+      <c r="B59" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="C59" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="D59" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="E59" s="22"/>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60" s="34" t="s">
+        <v>24</v>
+      </c>
+      <c r="B60" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="C60" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="D60" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="E60" s="22" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61" s="34" t="s">
+        <v>24</v>
+      </c>
+      <c r="B61" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="C61" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="D61" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="E61" s="22" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62" s="34"/>
+      <c r="B62" s="22"/>
+      <c r="C62" s="22"/>
+      <c r="D62" s="34"/>
+      <c r="E62" s="22"/>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="C52" s="3" t="s">
+      <c r="B63" s="26"/>
+      <c r="C63" s="26"/>
+      <c r="D63" s="26"/>
+      <c r="E63" s="27"/>
+    </row>
+    <row r="64" spans="1:5" ht="28.8">
+      <c r="A64" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B64" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C64" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="D64" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="E64" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5">
+      <c r="A65" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="B65" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C65" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D65" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="E65" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5">
+      <c r="B66" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C66" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D66" s="20" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5">
+      <c r="A68" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="B68" s="26"/>
+      <c r="C68" s="26"/>
+      <c r="D68" s="26"/>
+      <c r="E68" s="27"/>
+    </row>
+    <row r="69" spans="1:5" ht="28.8">
+      <c r="A69" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B69" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C69" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="D69" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="E69" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5">
+      <c r="A70" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B70" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="D52" s="33" t="s">
-        <v>7</v>
-      </c>
-      <c r="E52" s="3"/>
-    </row>
-    <row r="53" spans="1:5">
-      <c r="A53" s="33"/>
-      <c r="B53" s="3" t="s">
+      <c r="C70" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="D70" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E70" s="18" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5">
+      <c r="A71" s="24"/>
+      <c r="B71" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C71" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D71" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="E71" s="3"/>
+    </row>
+    <row r="72" spans="1:5">
+      <c r="A72" s="24"/>
+      <c r="B72" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C72" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D72" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="E72" s="3"/>
+    </row>
+    <row r="73" spans="1:5">
+      <c r="A73" s="24"/>
+      <c r="B73" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C73" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D73" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="E73" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5">
+      <c r="A74" s="24"/>
+      <c r="B74" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C74" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D74" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="E74" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5">
+      <c r="A75" s="24"/>
+      <c r="B75" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C53" s="3" t="s">
+      <c r="C75" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D75" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="E75" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5">
+      <c r="A76" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="B76" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C76" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D53" s="33" t="s">
-        <v>7</v>
-      </c>
-      <c r="E53" s="3"/>
-    </row>
-    <row r="54" spans="1:5">
-      <c r="A54" s="33"/>
-      <c r="B54" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C54" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D54" s="33" t="s">
-        <v>7</v>
-      </c>
-      <c r="E54" s="3" t="s">
+      <c r="D76" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="E76" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="55" spans="1:5">
-      <c r="A55" s="33"/>
-      <c r="B55" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C55" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="D55" s="33" t="s">
-        <v>7</v>
-      </c>
-      <c r="E55" s="3"/>
-    </row>
-    <row r="56" spans="1:5">
-      <c r="A56" s="33"/>
-      <c r="B56" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C56" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D56" s="33" t="s">
-        <v>7</v>
-      </c>
-      <c r="E56" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5">
-      <c r="A57" s="33" t="s">
+    <row r="77" spans="1:5">
+      <c r="A77" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="B57" s="3" t="s">
+      <c r="B77" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C57" s="3" t="s">
+      <c r="C77" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D57" s="33" t="s">
-        <v>7</v>
-      </c>
-      <c r="E57" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5">
-      <c r="A58" s="33" t="s">
-        <v>24</v>
-      </c>
-      <c r="B58" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C58" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D58" s="33" t="s">
-        <v>7</v>
-      </c>
-      <c r="E58" s="3" t="s">
-        <v>49</v>
+      <c r="D77" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="E77" s="3" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="13">
     <mergeCell ref="A32:E32"/>
     <mergeCell ref="A41:E41"/>
-    <mergeCell ref="A49:E49"/>
+    <mergeCell ref="A68:E68"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="A4:E4"/>
@@ -1648,6 +1933,9 @@
     <mergeCell ref="A15:E15"/>
     <mergeCell ref="A20:E20"/>
     <mergeCell ref="A26:E26"/>
+    <mergeCell ref="A63:E63"/>
+    <mergeCell ref="A54:E54"/>
+    <mergeCell ref="A49:E49"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.2" right="0.2" top="0.74803149606299202" bottom="0.74803149606299202" header="0.31496062992126" footer="0.31496062992126"/>

</xml_diff>